<commit_message>
paper edits and updated Wilcoxon within plant PAIRS
</commit_message>
<xml_diff>
--- a/paper/Results/CandidateLists_geneandSNP.xlsx
+++ b/paper/Results/CandidateLists_geneandSNP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="7635" windowHeight="3405" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="7635" windowHeight="3405" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="12plant_SNP" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Genotype</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>See venn_genes</t>
+  </si>
+  <si>
+    <t>Top 1000 SNPs only</t>
   </si>
 </sst>
 </file>
@@ -439,21 +442,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -478,11 +481,11 @@
         <v>629</v>
       </c>
       <c r="D2">
-        <f>SUM(B2:C2)</f>
+        <f t="shared" ref="D2:D13" si="0">SUM(B2:C2)</f>
         <v>1284</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -493,11 +496,11 @@
         <v>1300</v>
       </c>
       <c r="D3">
-        <f>SUM(B3:C3)</f>
+        <f t="shared" si="0"/>
         <v>2570</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -508,11 +511,11 @@
         <v>4441</v>
       </c>
       <c r="D4">
-        <f>SUM(B4:C4)</f>
+        <f t="shared" si="0"/>
         <v>7629</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -523,11 +526,11 @@
         <v>6034</v>
       </c>
       <c r="D5">
-        <f>SUM(B5:C5)</f>
+        <f t="shared" si="0"/>
         <v>8973</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -538,11 +541,11 @@
         <v>5859</v>
       </c>
       <c r="D6">
-        <f>SUM(B6:C6)</f>
+        <f t="shared" si="0"/>
         <v>10060</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -553,11 +556,11 @@
         <v>6237</v>
       </c>
       <c r="D7">
-        <f>SUM(B7:C7)</f>
+        <f t="shared" si="0"/>
         <v>10440</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -568,11 +571,11 @@
         <v>10427</v>
       </c>
       <c r="D8">
-        <f>SUM(B8:C8)</f>
+        <f t="shared" si="0"/>
         <v>16644</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -583,11 +586,11 @@
         <v>9915</v>
       </c>
       <c r="D9">
-        <f>SUM(B9:C9)</f>
+        <f t="shared" si="0"/>
         <v>16761</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -598,11 +601,11 @@
         <v>12340</v>
       </c>
       <c r="D10">
-        <f>SUM(B10:C10)</f>
+        <f t="shared" si="0"/>
         <v>21604</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -613,11 +616,11 @@
         <v>12190</v>
       </c>
       <c r="D11">
-        <f>SUM(B11:C11)</f>
+        <f t="shared" si="0"/>
         <v>21621</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -628,11 +631,11 @@
         <v>13877</v>
       </c>
       <c r="D12">
-        <f>SUM(B12:C12)</f>
+        <f t="shared" si="0"/>
         <v>25195</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -643,13 +646,114 @@
         <v>12774</v>
       </c>
       <c r="D13">
-        <f>SUM(B13:C13)</f>
+        <f t="shared" si="0"/>
         <v>25421</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f>SUM(D2:D13)</f>
+        <v>168202</v>
+      </c>
+      <c r="E14">
+        <f>46000/D14</f>
+        <v>0.27348069583001389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>9</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6564</v>
+      </c>
+      <c r="B20">
+        <v>1264</v>
+      </c>
+      <c r="C20">
+        <v>416</v>
+      </c>
+      <c r="D20">
+        <v>205</v>
+      </c>
+      <c r="E20">
+        <v>75</v>
+      </c>
+      <c r="F20">
+        <v>24</v>
+      </c>
+      <c r="G20">
+        <v>34</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f>SUM(A20:J20)</f>
+        <v>8592</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f>A20/K20</f>
+        <v>0.76396648044692739</v>
       </c>
     </row>
   </sheetData>
@@ -680,10 +784,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,17 +796,17 @@
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -743,7 +847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -783,9 +887,17 @@
       <c r="M7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="1">
+        <f>SUM(B7:M7)</f>
+        <v>990</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
+      <c r="N8" s="1">
+        <f>555/990</f>
+        <v>0.56060606060606055</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -797,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
paper updates and GEMMA/ bigRR overlap
</commit_message>
<xml_diff>
--- a/paper/Results/CandidateLists_geneandSNP.xlsx
+++ b/paper/Results/CandidateLists_geneandSNP.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesol\Documents\Projects\BcSolGWAS\paper\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2A9C1F-FC0A-4D81-9351-BDEFD54DF705}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="7635" windowHeight="3405"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="7640" windowHeight="3410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12plant_SNP" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
     <sheet name="12plant_gene" sheetId="3" r:id="rId3"/>
     <sheet name="Domest_gene" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -97,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,6 +160,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -201,7 +210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,9 +243,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,6 +295,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -444,22 +487,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="A18" sqref="A18:L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -488,7 +531,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -503,7 +546,7 @@
         <v>2570</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -518,7 +561,7 @@
         <v>7629</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -533,7 +576,7 @@
         <v>8973</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -548,7 +591,7 @@
         <v>10060</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -563,7 +606,7 @@
         <v>10440</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -578,7 +621,7 @@
         <v>16644</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -593,7 +636,7 @@
         <v>16761</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -608,7 +651,7 @@
         <v>21604</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -623,7 +666,7 @@
         <v>21621</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -638,7 +681,7 @@
         <v>25195</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -653,7 +696,7 @@
         <v>25421</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D14">
         <f>SUM(D2:D13)</f>
         <v>168202</v>
@@ -663,12 +706,12 @@
         <v>0.27348069583001389</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -679,7 +722,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>1</v>
       </c>
@@ -717,7 +760,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>46151</v>
       </c>
@@ -755,7 +798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -764,7 +807,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1</v>
       </c>
@@ -796,7 +839,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>6564</v>
       </c>
@@ -832,7 +875,7 @@
         <v>8592</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="K25">
         <f>A24/K24</f>
         <v>0.76396648044692739</v>
@@ -848,14 +891,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -866,30 +909,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="41.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -930,7 +973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -975,7 +1018,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="N8" s="1">
         <f>555/990</f>
@@ -989,16 +1032,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>

</xml_diff>